<commit_message>
Taxis im Modell statt aus DB
</commit_message>
<xml_diff>
--- a/IT-Projekt/data_v1.xlsx
+++ b/IT-Projekt/data_v1.xlsx
@@ -5,17 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lars\Desktop\IT-Projekt-Anylogic\IT-Projekt\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikla\Documents\GitHub\IT-Projekt-Anylogic\IT-Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96267B2-3353-40CD-B08A-4BC40219CB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AD6BB8-4729-4106-90F0-19260B8AFDB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
     <sheet name="TaxiStands" sheetId="2" r:id="rId2"/>
-    <sheet name="Taxis" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,28 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
-  <si>
-    <t>Tesla</t>
-  </si>
-  <si>
-    <t>DestLat</t>
-  </si>
-  <si>
-    <t>DestLong</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>batteryCapacity</t>
-  </si>
-  <si>
-    <t>maxRange</t>
-  </si>
-  <si>
-    <t>currentRange</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>locationLat</t>
   </si>
@@ -413,36 +391,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>120</v>
       </c>
@@ -460,7 +438,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>120</v>
       </c>
@@ -477,7 +455,7 @@
         <v>9.7309718027690906</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>120</v>
       </c>
@@ -494,7 +472,7 @@
         <v>9.7309718027690906</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>120</v>
       </c>
@@ -511,7 +489,7 @@
         <v>9.7309718027690906</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>120</v>
       </c>
@@ -528,7 +506,7 @@
         <v>9.7309718027690906</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>120</v>
       </c>
@@ -545,7 +523,7 @@
         <v>9.7309718027690906</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>120</v>
       </c>
@@ -562,7 +540,7 @@
         <v>9.7309718027690906</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>120</v>
       </c>
@@ -579,7 +557,7 @@
         <v>9.7309718027690906</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>120</v>
       </c>
@@ -597,7 +575,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>120</v>
       </c>
@@ -615,7 +593,7 @@
       </c>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>120</v>
       </c>
@@ -633,7 +611,7 @@
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>120</v>
       </c>
@@ -651,7 +629,7 @@
       </c>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>120</v>
       </c>
@@ -669,7 +647,7 @@
       </c>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>120</v>
       </c>
@@ -687,7 +665,7 @@
       </c>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>120</v>
       </c>
@@ -705,7 +683,7 @@
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>120</v>
       </c>
@@ -737,29 +715,29 @@
       <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>52.386400000000002</v>
       </c>
@@ -776,7 +754,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>52.389690000000002</v>
       </c>
@@ -793,7 +771,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>52.381039999999999</v>
       </c>
@@ -810,7 +788,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>52.37323</v>
       </c>
@@ -827,7 +805,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>52.373089999999998</v>
       </c>
@@ -844,7 +822,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>52.380740000000003</v>
       </c>
@@ -861,7 +839,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>52.366759999999999</v>
       </c>
@@ -878,7 +856,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>52.373089999999998</v>
       </c>
@@ -895,7 +873,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>52.390889999999999</v>
       </c>
@@ -912,7 +890,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>52.397959999999998</v>
       </c>
@@ -929,7 +907,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>52.374769999999998</v>
       </c>
@@ -946,7 +924,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>52.365789999999997</v>
       </c>
@@ -963,7 +941,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>52.364780000000003</v>
       </c>
@@ -980,7 +958,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>52.37377</v>
       </c>
@@ -997,7 +975,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>52.386130000000001</v>
       </c>
@@ -1014,7 +992,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>52.399000000000001</v>
       </c>
@@ -1031,7 +1009,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>52.366669999999999</v>
       </c>
@@ -1048,7 +1026,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>52.359400000000001</v>
       </c>
@@ -1065,7 +1043,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>52.364429999999999</v>
       </c>
@@ -1082,7 +1060,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>52.381419999999999</v>
       </c>
@@ -1099,7 +1077,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>52.356819999999999</v>
       </c>
@@ -1116,7 +1094,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>52.365400000000001</v>
       </c>
@@ -1133,7 +1111,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>52.349710000000002</v>
       </c>
@@ -1150,7 +1128,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>52.399050000000003</v>
       </c>
@@ -1167,7 +1145,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>52.397950000000002</v>
       </c>
@@ -1182,147 +1160,6 @@
       </c>
       <c r="E26" s="3">
         <v>200</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C51E590-80CB-4323-97E0-0D589D623D52}">
-  <dimension ref="A1:G6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:G6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>52.381989108834198</v>
-      </c>
-      <c r="B2" s="2">
-        <v>9.7401182223916098</v>
-      </c>
-      <c r="D2">
-        <v>3000000</v>
-      </c>
-      <c r="E2">
-        <v>3000000</v>
-      </c>
-      <c r="F2">
-        <v>30000</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>52.389690000000002</v>
-      </c>
-      <c r="B3" s="4">
-        <v>9.7207399999999993</v>
-      </c>
-      <c r="D3">
-        <v>3000000</v>
-      </c>
-      <c r="E3">
-        <v>3000000</v>
-      </c>
-      <c r="F3">
-        <v>30000</v>
-      </c>
-      <c r="G3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>52.381989108834198</v>
-      </c>
-      <c r="B4" s="4">
-        <v>9.7401182223916098</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3">
-        <v>3000000</v>
-      </c>
-      <c r="E4" s="3">
-        <v>3000000</v>
-      </c>
-      <c r="F4" s="3">
-        <v>30000</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>52.389690000000002</v>
-      </c>
-      <c r="B5" s="4">
-        <v>9.7207399999999993</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3">
-        <v>3000000</v>
-      </c>
-      <c r="E5" s="3">
-        <v>3000000</v>
-      </c>
-      <c r="F5" s="3">
-        <v>30000</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>52.389690000000002</v>
-      </c>
-      <c r="B6" s="4">
-        <v>9.7207399999999993</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3">
-        <v>3000000</v>
-      </c>
-      <c r="E6" s="3">
-        <v>3000000</v>
-      </c>
-      <c r="F6" s="3">
-        <v>30000</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>